<commit_message>
listo par revision d equipos items
</commit_message>
<xml_diff>
--- a/productividad equpos3.xlsx
+++ b/productividad equpos3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="15600" windowHeight="7995" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15600" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="excavadoras" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="173">
   <si>
     <t>PRODUCTIVIDAD</t>
   </si>
@@ -552,6 +552,24 @@
   </si>
   <si>
     <t>m3/hora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RETROEXCAVADORA </t>
+  </si>
+  <si>
+    <t>CAT 428 F</t>
+  </si>
+  <si>
+    <t>factor cucharon</t>
+  </si>
+  <si>
+    <t>factor material</t>
+  </si>
+  <si>
+    <t>eficiencia de trabajo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productividad real promedio </t>
   </si>
 </sst>
 </file>
@@ -622,7 +640,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -630,32 +648,129 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,159 +1072,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="B3" s="18"/>
+      <c r="C3" s="21">
         <f>G3*60/G6</f>
         <v>142.85714285714286</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="18">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G4">
+      <c r="F4" s="18"/>
+      <c r="G4" s="18">
         <v>90</v>
       </c>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G5">
+      <c r="F5" s="18"/>
+      <c r="G5" s="18">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="18">
         <v>0.42</v>
       </c>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="18">
         <v>0.42</v>
       </c>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18">
         <f>G3*60*H11*G12*G10/G8</f>
         <v>85.714285714285722</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="18">
         <v>0</v>
       </c>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="18">
         <v>1</v>
       </c>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F11" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="18">
         <v>1.5</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="19">
         <f>1/1.5</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="23">
         <v>0.9</v>
       </c>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="21">
+        <f>G17*60/G20</f>
+        <v>142.85714285714286</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="18">
+        <v>1</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18">
+        <v>90</v>
+      </c>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18">
+        <v>1</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0.42</v>
+      </c>
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0.42</v>
+      </c>
+      <c r="H22" s="19"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18">
+        <f>G17*60*H25*G26*G24/G22</f>
+        <v>85.714285714285722</v>
+      </c>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="18">
+        <v>0</v>
+      </c>
+      <c r="H23" s="19"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="18">
+        <v>1</v>
+      </c>
+      <c r="H24" s="19"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="H25" s="19">
+        <f>1/1.5</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="H26" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1138,10 +1523,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="10"/>
       <c r="C2" t="s">
         <v>12</v>
       </c>
@@ -1470,10 +1855,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="10"/>
       <c r="C2" t="s">
         <v>12</v>
       </c>
@@ -1721,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,22 +2121,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="10"/>
       <c r="C2" t="s">
         <v>12</v>
       </c>
@@ -1818,7 +2203,7 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="11" t="s">
         <v>66</v>
       </c>
       <c r="F7" t="s">
@@ -1837,7 +2222,7 @@
         <f>G7*G9</f>
         <v>7.8947368421052637</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
@@ -2114,22 +2499,22 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="9"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="10"/>
       <c r="C31" t="s">
         <v>12</v>
       </c>
@@ -2190,7 +2575,7 @@
       <c r="C36" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="11" t="s">
         <v>66</v>
       </c>
       <c r="F36" t="s">
@@ -2209,7 +2594,7 @@
         <f>G36*G38</f>
         <v>7.8947368421052637</v>
       </c>
-      <c r="E37" s="7"/>
+      <c r="E37" s="11"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
@@ -2483,6 +2868,20 @@
       </c>
       <c r="G56">
         <v>0.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>172</v>
+      </c>
+      <c r="B59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <f>AVERAGE(C53,C24)</f>
+        <v>71.059153317643634</v>
       </c>
     </row>
   </sheetData>
@@ -2503,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,10 +2924,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="10"/>
       <c r="C2" t="s">
         <v>114</v>
       </c>
@@ -2557,7 +2956,7 @@
       <c r="H3" t="s">
         <v>114</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="8" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2710,7 +3109,7 @@
       <c r="F14" t="s">
         <v>128</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="7">
         <v>30</v>
       </c>
       <c r="I14" t="s">
@@ -2722,7 +3121,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="G15" s="10"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2740,7 +3139,7 @@
       <c r="F16" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="7">
         <v>100</v>
       </c>
       <c r="H16" t="s">
@@ -2815,7 +3214,7 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>114</v>
       </c>
       <c r="E22" t="s">
         <v>140</v>
@@ -2882,8 +3281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2901,10 +3300,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="10"/>
       <c r="C2" t="s">
         <v>114</v>
       </c>
@@ -3058,10 +3457,10 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="10"/>
       <c r="C18" t="s">
         <v>114</v>
       </c>
@@ -3121,7 +3520,7 @@
       <c r="F21" t="s">
         <v>155</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="9">
         <f>I21/1000</f>
         <v>2.13</v>
       </c>
@@ -3173,6 +3572,7 @@
       <c r="F27" t="s">
         <v>161</v>
       </c>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">

</xml_diff>